<commit_message>
Updating codes till 11/10/24
</commit_message>
<xml_diff>
--- a/Leet Code/Revision Status.xlsx
+++ b/Leet Code/Revision Status.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HARSHAL\Desktop\Leet Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEC0B2B-BF7A-49E7-994D-52ABFE440C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623CB46D-D8B1-4F9B-8728-E801B6AAB630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3CDF1EAA-ABD8-4982-AE85-2C9F7C7D98F7}"/>
+    <workbookView minimized="1" xWindow="1170" yWindow="680" windowWidth="14400" windowHeight="7270" xr2:uid="{3CDF1EAA-ABD8-4982-AE85-2C9F7C7D98F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Leetcode" sheetId="1" r:id="rId1"/>
@@ -518,104 +518,110 @@
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C3" s="1">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C4" s="1">
-        <v>152</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2</v>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C5" s="1">
-        <v>162</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C6" s="1">
-        <v>169</v>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C7" s="1">
-        <v>268</v>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C8" s="1">
-        <v>349</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C9" s="1">
-        <v>367</v>
+        <v>445</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C10" s="1">
-        <v>852</v>
+        <v>496</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C11" s="1">
-        <v>875</v>
+        <v>503</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C12" s="1">
-        <v>1011</v>
+        <v>556</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -623,70 +629,76 @@
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C13" s="1">
-        <v>1237</v>
+        <v>1019</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C14" s="1">
-        <v>1337</v>
+        <v>1385</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C15" s="1">
-        <v>1351</v>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C16" s="1">
-        <v>1552</v>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C17" s="1">
-        <v>2089</v>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C18" s="1">
-        <v>2389</v>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C19" s="1">
-        <v>2824</v>
+      <c r="C19" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -694,10 +706,10 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -705,18 +717,18 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C21" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C22" s="1" t="s">
-        <v>21</v>
+      <c r="C22" s="1">
+        <v>34</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -726,30 +738,30 @@
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C23" s="1" t="s">
-        <v>23</v>
+      <c r="C23" s="1">
+        <v>152</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C24" s="1" t="s">
-        <v>25</v>
+      <c r="C24" s="1">
+        <v>162</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C25" s="1" t="s">
-        <v>31</v>
+      <c r="C25" s="1">
+        <v>169</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -760,7 +772,7 @@
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
-        <v>719</v>
+        <v>268</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -771,54 +783,48 @@
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
-        <v>4</v>
+        <v>349</v>
       </c>
       <c r="D27" s="1">
-        <v>2</v>
-      </c>
-      <c r="E27" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
-        <v>445</v>
+        <v>367</v>
       </c>
       <c r="D28" s="1">
-        <v>2</v>
-      </c>
-      <c r="E28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
-        <v>496</v>
+        <v>852</v>
       </c>
       <c r="D29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
-        <v>503</v>
+        <v>875</v>
       </c>
       <c r="D30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
-        <v>556</v>
+        <v>1011</v>
       </c>
       <c r="D31" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -826,76 +832,70 @@
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
-        <v>1019</v>
+        <v>1237</v>
       </c>
       <c r="D32" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
-        <v>1385</v>
+        <v>1337</v>
       </c>
       <c r="D33" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C34" s="1" t="s">
-        <v>20</v>
+      <c r="C34" s="1">
+        <v>1351</v>
       </c>
       <c r="D34" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C35" s="1" t="s">
-        <v>27</v>
+      <c r="C35" s="1">
+        <v>1552</v>
       </c>
       <c r="D35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C36" s="1" t="s">
-        <v>19</v>
+      <c r="C36" s="1">
+        <v>2089</v>
       </c>
       <c r="D36" s="1">
-        <v>2</v>
-      </c>
-      <c r="E36" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C37" s="1" t="s">
-        <v>26</v>
+      <c r="C37" s="1">
+        <v>2389</v>
       </c>
       <c r="D37" s="1">
-        <v>2</v>
-      </c>
-      <c r="E37" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C38" s="1" t="s">
-        <v>3</v>
+      <c r="C38" s="1">
+        <v>2824</v>
       </c>
       <c r="D38" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -903,10 +903,10 @@
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C39" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D39" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -914,21 +914,21 @@
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C40" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D40" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C41" s="1">
-        <v>53</v>
+      <c r="C41" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D41" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -936,21 +936,21 @@
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C42" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D42" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C43" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D43" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
@@ -958,24 +958,24 @@
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>30</v>
+      <c r="C45" s="1">
+        <v>719</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.35">
@@ -991,8 +991,8 @@
     </row>
   </sheetData>
   <autoFilter ref="C2:E44" xr:uid="{D0D62A89-97A0-4713-91F2-693EBE1F7336}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:E45">
-      <sortCondition ref="D2:D44"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:E46">
+      <sortCondition descending="1" ref="D2:D44"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>